<commit_message>
Adding research and database toolsets
</commit_message>
<xml_diff>
--- a/sources.xlsx
+++ b/sources.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanstruk/Documents/GitHub/good-news/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB113C-8DFC-D049-BE97-ADA9808F317F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5D5AD3-6667-3842-91C1-04A069227C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42480" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
+    <workbookView xWindow="42480" yWindow="3200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AC684F59-F628-C54A-AD30-D4C8ABAC84A6}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
+    <sheet name="blocked_domains" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sources!$C$1:$F$1</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>RSS</t>
   </si>
@@ -140,6 +141,15 @@
   </si>
   <si>
     <t>desc_topic_primary</t>
+  </si>
+  <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>finance.yahoo.com</t>
+  </si>
+  <si>
+    <t>bloomberg.com</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E55AEB-D2F4-EE41-86F8-038347F2C987}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1300,4 +1310,34 @@
   <autoFilter ref="C1:F1" xr:uid="{19E55AEB-D2F4-EE41-86F8-038347F2C987}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A4B157-2370-6347-AE30-C440E2E17D8E}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>